<commit_message>
Boss's edits: recruitment totals, Christmas Day text, font readability
1. Updated recruitment counts from "Total Randomised" column in spreadsheet
   - Now shows actual recruitment numbers (e.g., Arizona: 200, Charite: 102)
   - Changed text to "X recruited so far"

2. Changed "Xmas Eve" to "Christmas Day" in grand prize info card

3. Improved gift box font readability:
   - Increased font size for date and center count
   - Added stronger drop shadows (multiple layers)
   - Made text bold (font-weight: 600)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/12Days_of_CARSK_BRG.xlsx
+++ b/assets/12Days_of_CARSK_BRG.xlsx
@@ -1,45 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VCHAhome1.vch.ca\briougreen-INFOSYS\Profile\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavgay\Desktop\CARSK_advent_calendar\carsk_advent_calendar\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9905C3F2-08DF-44CB-91BF-21038BDA0FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96E75D0-4512-4E32-9619-D1B0B1366778}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D27FD18B-B50C-49A5-8F72-C3BDE24D7A7C}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" xr2:uid="{D27FD18B-B50C-49A5-8F72-C3BDE24D7A7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="135">
   <si>
     <t>Center</t>
   </si>
@@ -441,6 +430,9 @@
   </si>
   <si>
     <t xml:space="preserve">Team players  !                                                                                                                                   CARSK is an international study with some sites as close at 4 km apart! These sites have accepted a transfer of a research patients so they can continue in the trial in their randomization arm. </t>
+  </si>
+  <si>
+    <t>Total Randomised</t>
   </si>
 </sst>
 </file>
@@ -508,9 +500,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -548,7 +540,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -654,7 +646,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -796,7 +788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -804,23 +796,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9EC511-B106-4564-8D8D-B7A2A62608DF}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" customWidth="1"/>
-    <col min="6" max="6" width="48.453125" customWidth="1"/>
+    <col min="2" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,1500 +820,1725 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
         <v>99</v>
       </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
         <v>98</v>
       </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>110</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>110</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>6</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
         <v>96</v>
       </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>6</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>11</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15">
         <v>11</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16">
         <v>11</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>11</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18">
         <v>3</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>3</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
         <v>100</v>
       </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22">
         <v>8</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23">
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>8</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24">
         <v>9</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
         <v>101</v>
       </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25">
         <v>9</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
         <v>36</v>
       </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <v>9</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
         <v>37</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>102</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>9</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
         <v>103</v>
       </c>
-      <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28">
         <v>3</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
         <v>39</v>
       </c>
-      <c r="D29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>3</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
         <v>104</v>
       </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30">
         <v>4</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="D31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>4</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
       <c r="B32" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32">
+        <v>71</v>
+      </c>
+      <c r="D32" t="s">
         <v>44</v>
       </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32">
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32">
         <v>3</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
         <v>45</v>
       </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33">
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>3</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
       <c r="B34" t="s">
         <v>46</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
         <v>48</v>
       </c>
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34">
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34">
         <v>4</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
       <c r="B35" t="s">
         <v>46</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
         <v>49</v>
       </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35">
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35">
         <v>4</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" t="s">
         <v>46</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
         <v>50</v>
       </c>
-      <c r="D36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36">
+      <c r="E36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>4</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37">
+        <v>200</v>
+      </c>
+      <c r="D37" t="s">
         <v>52</v>
       </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37">
+      <c r="E37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>12</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
       <c r="B38" t="s">
         <v>46</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38">
+        <v>200</v>
+      </c>
+      <c r="D38" t="s">
         <v>53</v>
       </c>
-      <c r="D38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38">
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38">
         <v>12</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
         <v>55</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>110</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>10</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
       <c r="B40" t="s">
         <v>46</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
         <v>56</v>
       </c>
-      <c r="D40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40">
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40">
         <v>10</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
         <v>57</v>
       </c>
-      <c r="D41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41">
+      <c r="E41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>10</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
         <v>59</v>
       </c>
-      <c r="D42" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42">
+      <c r="E42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42">
         <v>10</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
         <v>106</v>
       </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43">
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43">
         <v>10</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>46</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
         <v>105</v>
       </c>
-      <c r="D44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44">
         <v>10</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
         <v>60</v>
       </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45">
+      <c r="E45" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45">
         <v>10</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
       <c r="B46" t="s">
         <v>46</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46">
+        <v>31</v>
+      </c>
+      <c r="D46" t="s">
         <v>107</v>
       </c>
-      <c r="D46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E46">
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46">
         <v>6</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47">
+        <v>31</v>
+      </c>
+      <c r="D47" t="s">
         <v>62</v>
       </c>
-      <c r="D47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47">
+      <c r="E47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47">
         <v>6</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
         <v>64</v>
       </c>
-      <c r="D48" t="s">
-        <v>2</v>
-      </c>
-      <c r="E48">
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48">
         <v>9</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
         <v>65</v>
       </c>
-      <c r="D49" t="s">
-        <v>2</v>
-      </c>
-      <c r="E49">
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49">
         <v>9</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
       <c r="B50" t="s">
         <v>46</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
         <v>66</v>
       </c>
-      <c r="D50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50">
+      <c r="E50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50">
         <v>9</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>68</v>
       </c>
       <c r="B51" t="s">
         <v>67</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51">
+        <v>32</v>
+      </c>
+      <c r="D51" t="s">
         <v>69</v>
       </c>
-      <c r="D51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51">
+      <c r="E51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51">
         <v>7</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>68</v>
       </c>
       <c r="B52" t="s">
         <v>67</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52">
+        <v>32</v>
+      </c>
+      <c r="D52" t="s">
         <v>108</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>102</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>7</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
       <c r="B53" t="s">
         <v>67</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s">
         <v>70</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>110</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>7</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>68</v>
       </c>
       <c r="B54" t="s">
         <v>67</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54">
+        <v>32</v>
+      </c>
+      <c r="D54" t="s">
         <v>109</v>
       </c>
-      <c r="D54" t="s">
-        <v>2</v>
-      </c>
-      <c r="E54">
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54">
         <v>7</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>72</v>
       </c>
       <c r="B55" t="s">
         <v>71</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55">
+        <v>102</v>
+      </c>
+      <c r="D55" t="s">
         <v>111</v>
       </c>
-      <c r="D55" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55">
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55">
         <v>7</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>72</v>
       </c>
       <c r="B56" t="s">
         <v>71</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56">
+        <v>102</v>
+      </c>
+      <c r="D56" t="s">
         <v>112</v>
       </c>
-      <c r="D56" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56">
+      <c r="E56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56">
         <v>7</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>74</v>
       </c>
       <c r="B57" t="s">
         <v>73</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57">
+        <v>17</v>
+      </c>
+      <c r="D57" t="s">
         <v>75</v>
       </c>
-      <c r="D57" t="s">
-        <v>1</v>
-      </c>
-      <c r="E57">
+      <c r="E57" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57">
         <v>5</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
       <c r="B58" t="s">
         <v>73</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58">
+        <v>17</v>
+      </c>
+      <c r="D58" t="s">
         <v>76</v>
       </c>
-      <c r="D58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E58">
+      <c r="E58" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58">
         <v>5</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>77</v>
       </c>
       <c r="B59" t="s">
         <v>73</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59">
+        <v>40</v>
+      </c>
+      <c r="D59" t="s">
         <v>78</v>
       </c>
-      <c r="D59" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59">
+      <c r="E59" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59">
         <v>5</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>77</v>
       </c>
       <c r="B60" t="s">
         <v>73</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60">
+        <v>40</v>
+      </c>
+      <c r="D60" t="s">
         <v>79</v>
       </c>
-      <c r="D60" t="s">
-        <v>2</v>
-      </c>
-      <c r="E60">
+      <c r="E60" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60">
         <v>5</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>77</v>
       </c>
       <c r="B61" t="s">
         <v>73</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61">
+        <v>40</v>
+      </c>
+      <c r="D61" t="s">
         <v>80</v>
       </c>
-      <c r="D61" t="s">
-        <v>2</v>
-      </c>
-      <c r="E61">
+      <c r="E61" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61">
         <v>5</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>81</v>
       </c>
       <c r="B62" t="s">
         <v>73</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62">
+        <v>90</v>
+      </c>
+      <c r="D62" t="s">
         <v>113</v>
       </c>
-      <c r="D62" t="s">
-        <v>1</v>
-      </c>
-      <c r="E62">
-        <v>2</v>
-      </c>
-      <c r="F62" s="2" t="s">
+      <c r="E62" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>81</v>
       </c>
       <c r="B63" t="s">
         <v>73</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63">
+        <v>90</v>
+      </c>
+      <c r="D63" t="s">
         <v>120</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>114</v>
       </c>
-      <c r="E63">
-        <v>2</v>
-      </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>81</v>
       </c>
       <c r="B64" t="s">
         <v>73</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64">
+        <v>90</v>
+      </c>
+      <c r="D64" t="s">
         <v>119</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>114</v>
       </c>
-      <c r="E64">
-        <v>2</v>
-      </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
       <c r="B65" t="s">
         <v>73</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65">
+        <v>31</v>
+      </c>
+      <c r="D65" t="s">
         <v>83</v>
       </c>
-      <c r="D65" t="s">
-        <v>1</v>
-      </c>
-      <c r="E65">
+      <c r="E65" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65">
         <v>4</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
       <c r="B66" t="s">
         <v>73</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66">
+        <v>31</v>
+      </c>
+      <c r="D66" t="s">
         <v>117</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>114</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>4</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>84</v>
       </c>
       <c r="B67" t="s">
         <v>73</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67">
+        <v>27</v>
+      </c>
+      <c r="D67" t="s">
         <v>116</v>
       </c>
-      <c r="D67" t="s">
-        <v>1</v>
-      </c>
-      <c r="E67">
+      <c r="E67" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67">
         <v>11</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>84</v>
       </c>
       <c r="B68" t="s">
         <v>73</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68">
+        <v>27</v>
+      </c>
+      <c r="D68" t="s">
         <v>118</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>114</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>11</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>85</v>
       </c>
       <c r="B69" t="s">
         <v>73</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69">
+        <v>30</v>
+      </c>
+      <c r="D69" t="s">
         <v>86</v>
       </c>
-      <c r="D69" t="s">
-        <v>1</v>
-      </c>
-      <c r="E69">
+      <c r="E69" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69">
         <v>4</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>85</v>
       </c>
       <c r="B70" t="s">
         <v>73</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70">
+        <v>30</v>
+      </c>
+      <c r="D70" t="s">
         <v>87</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>114</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>4</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>
       <c r="B71" t="s">
         <v>73</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
         <v>89</v>
       </c>
-      <c r="D71" t="s">
-        <v>1</v>
-      </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="E71" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>88</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
         <v>90</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>114</v>
       </c>
-      <c r="E72">
-        <v>2</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>91</v>
       </c>
       <c r="B73" t="s">
         <v>73</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73">
+        <v>65</v>
+      </c>
+      <c r="D73" t="s">
         <v>115</v>
       </c>
-      <c r="D73" t="s">
-        <v>1</v>
-      </c>
-      <c r="E73">
+      <c r="E73" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73">
         <v>9</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>91</v>
       </c>
       <c r="B74" t="s">
         <v>73</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74">
+        <v>65</v>
+      </c>
+      <c r="D74" t="s">
         <v>92</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>114</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>9</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>91</v>
       </c>
       <c r="B75" t="s">
         <v>73</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75">
+        <v>65</v>
+      </c>
+      <c r="D75" t="s">
         <v>93</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>114</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>9</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F75" xr:uid="{CB9EC511-B106-4564-8D8D-B7A2A62608DF}"/>
+  <autoFilter ref="A1:G75" xr:uid="{CB9EC511-B106-4564-8D8D-B7A2A62608DF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>